<commit_message>
1) Add natural language processing to compare data sheet value similiarity vs spec value, highlight the cells in "Similarity" column of "raw_datasheet" worksheet to green when similiarity exceed its predefined threshold of >=20%
2) NLP similarity algorithm is created base on NLP_Modules.py and called upon its function
</commit_message>
<xml_diff>
--- a/ref.xlsx
+++ b/ref.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YewLoung/PycharmProjects/SE_Datasheet_Scrape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C2E15B-D585-B04D-A8D8-6712DF17BA6A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434FE359-CE46-A84D-9277-8D4CD187C514}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="19520" windowHeight="12320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>RM17JC00MW</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>RSB2A080M7S</t>
+  </si>
+  <si>
+    <t>RXG11RD</t>
+  </si>
+  <si>
+    <t>RXM2AB1B7</t>
+  </si>
+  <si>
+    <t>RXM4AB1B7</t>
   </si>
 </sst>
 </file>
@@ -446,13 +455,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -539,6 +551,21 @@
         <v>16</v>
       </c>
     </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1) Add more color format 2) Add "X_Correction" col to each pivot datasheet ref 3) Clean format of "Raw_Datasheet" worksheet 4) Add "unique" and 'most_frequent" function 5) Add columns "count no of value", "count no of unique value", "count no most frequent value", "get all item list", 'get all unique list', ""get most frequent value" into pivot1 6) Copy "count no of unique value", "count no most frequent value", ""get most frequent value" from pivot1 to pivot 7) Solve the bug for converting and commercial to str type before combining into URL in order to take care those commercial is pure numeric number
</commit_message>
<xml_diff>
--- a/ref.xlsx
+++ b/ref.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YewLoung/PycharmProjects/SE_Datasheet_Scrape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434FE359-CE46-A84D-9277-8D4CD187C514}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FB412E-01EE-4C4F-AC17-9DDD187FBEC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="19520" windowHeight="12320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>RM17JC00MW</t>
-  </si>
-  <si>
     <t>RM17TA00</t>
   </si>
   <si>
@@ -34,52 +31,55 @@
     <t>RM10TE00</t>
   </si>
   <si>
-    <t>RE22R2AMR</t>
-  </si>
-  <si>
-    <t>RE22R2CMR</t>
-  </si>
-  <si>
-    <t>RMTJ60BD</t>
-  </si>
-  <si>
-    <t>XVDLS37</t>
-  </si>
-  <si>
-    <t>XVDLS38</t>
-  </si>
-  <si>
-    <t>RHT428B</t>
-  </si>
-  <si>
-    <t>RHT418BE</t>
-  </si>
-  <si>
-    <t>RSB1A160M7S</t>
-  </si>
-  <si>
-    <t>RSB1A160NDS</t>
-  </si>
-  <si>
-    <t>RSB2A080P7S</t>
-  </si>
-  <si>
-    <t>RSB2A080RDS</t>
-  </si>
-  <si>
-    <t>RSB2A080U7S</t>
-  </si>
-  <si>
-    <t>RSB2A080M7S</t>
-  </si>
-  <si>
-    <t>RXG11RD</t>
-  </si>
-  <si>
-    <t>RXM2AB1B7</t>
-  </si>
-  <si>
-    <t>RXM4AB1B7</t>
+    <t>RM22TG20</t>
+  </si>
+  <si>
+    <t>RM22TR33</t>
+  </si>
+  <si>
+    <t>RM22TR31</t>
+  </si>
+  <si>
+    <t>RM22TU23</t>
+  </si>
+  <si>
+    <t>RM22TU21</t>
+  </si>
+  <si>
+    <t>RM22TA33</t>
+  </si>
+  <si>
+    <t>RM22TA31</t>
+  </si>
+  <si>
+    <t>RM17TG20</t>
+  </si>
+  <si>
+    <t>RM17TG00</t>
+  </si>
+  <si>
+    <t>RM10TG00</t>
+  </si>
+  <si>
+    <t>RM17TU00</t>
+  </si>
+  <si>
+    <t>RM17TT00</t>
+  </si>
+  <si>
+    <t>RM35TF30</t>
+  </si>
+  <si>
+    <t>RM35TF30SP01</t>
+  </si>
+  <si>
+    <t>RM35UB330</t>
+  </si>
+  <si>
+    <t>RM35UB3N30</t>
+  </si>
+  <si>
+    <t>RM17UB310</t>
   </si>
 </sst>
 </file>
@@ -115,8 +115,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:B56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -467,103 +470,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>84873021</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>84873891</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>84873029</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>84873890</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>84873034</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>84873195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>84873025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>84873023</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>84873805</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>84873024</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>84873892</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>84873804</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>84873022</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>84873026</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>84873893</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>84873220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>84873894</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>84873221</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>84873895</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>84873222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>84873896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) remove https://www.schneider-electric.cn/en/product/<ref>/ , 'https://www.se.com/fr/en/product/<ref>/' url for web scraping 2) format col width of status worksheet 3) refactor code for conditional format pivot1 worksheet 4) add border line to whole table of pivot worksheet 5) add conditional red text to X_correction column when it is with text 6) successfully create conditional formatting using formula syntax construction method using xl_rowcol_to_cell() function
</commit_message>
<xml_diff>
--- a/ref.xlsx
+++ b/ref.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YewLoung/PycharmProjects/SE_Datasheet_Scrape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FB412E-01EE-4C4F-AC17-9DDD187FBEC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{434FE359-CE46-A84D-9277-8D4CD187C514}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="19520" windowHeight="12320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
+    <t>RM17JC00MW</t>
+  </si>
+  <si>
     <t>RM17TA00</t>
   </si>
   <si>
@@ -31,55 +34,52 @@
     <t>RM10TE00</t>
   </si>
   <si>
-    <t>RM22TG20</t>
-  </si>
-  <si>
-    <t>RM22TR33</t>
-  </si>
-  <si>
-    <t>RM22TR31</t>
-  </si>
-  <si>
-    <t>RM22TU23</t>
-  </si>
-  <si>
-    <t>RM22TU21</t>
-  </si>
-  <si>
-    <t>RM22TA33</t>
-  </si>
-  <si>
-    <t>RM22TA31</t>
-  </si>
-  <si>
-    <t>RM17TG20</t>
-  </si>
-  <si>
-    <t>RM17TG00</t>
-  </si>
-  <si>
-    <t>RM10TG00</t>
-  </si>
-  <si>
-    <t>RM17TU00</t>
-  </si>
-  <si>
-    <t>RM17TT00</t>
-  </si>
-  <si>
-    <t>RM35TF30</t>
-  </si>
-  <si>
-    <t>RM35TF30SP01</t>
-  </si>
-  <si>
-    <t>RM35UB330</t>
-  </si>
-  <si>
-    <t>RM35UB3N30</t>
-  </si>
-  <si>
-    <t>RM17UB310</t>
+    <t>RE22R2AMR</t>
+  </si>
+  <si>
+    <t>RE22R2CMR</t>
+  </si>
+  <si>
+    <t>RMTJ60BD</t>
+  </si>
+  <si>
+    <t>XVDLS37</t>
+  </si>
+  <si>
+    <t>XVDLS38</t>
+  </si>
+  <si>
+    <t>RHT428B</t>
+  </si>
+  <si>
+    <t>RHT418BE</t>
+  </si>
+  <si>
+    <t>RSB1A160M7S</t>
+  </si>
+  <si>
+    <t>RSB1A160NDS</t>
+  </si>
+  <si>
+    <t>RSB2A080P7S</t>
+  </si>
+  <si>
+    <t>RSB2A080RDS</t>
+  </si>
+  <si>
+    <t>RSB2A080U7S</t>
+  </si>
+  <si>
+    <t>RSB2A080M7S</t>
+  </si>
+  <si>
+    <t>RXG11RD</t>
+  </si>
+  <si>
+    <t>RXM2AB1B7</t>
+  </si>
+  <si>
+    <t>RXM4AB1B7</t>
   </si>
 </sst>
 </file>
@@ -115,11 +115,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A41"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -470,208 +467,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>84873021</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>84873891</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>84873029</v>
-      </c>
-    </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>84873890</v>
+      <c r="A14" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>84873034</v>
+      <c r="A15" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>84873195</v>
+      <c r="A16" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>1</v>
+      <c r="A17" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>2</v>
+      <c r="A18" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>84873025</v>
+      <c r="A19" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>84873023</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>84873805</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>84873024</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>84873892</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>84873804</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>84873022</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>84873026</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>84873893</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>84873220</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>84873894</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>84873221</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>84873895</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1" t="s">
+      <c r="A20" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>84873222</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>84873896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>